<commit_message>
UPDATES AND TROUBLE SHOOT ISSUES FOR RELATIVE VALUE STORED
</commit_message>
<xml_diff>
--- a/btc_blk_times.xlsx
+++ b/btc_blk_times.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3414"/>
+  <dimension ref="A1:E3415"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -58243,6 +58243,23 @@
         <v>-15.51439628096364</v>
       </c>
     </row>
+    <row r="3415">
+      <c r="A3415" s="1" t="n">
+        <v>3413</v>
+      </c>
+      <c r="B3415" t="n">
+        <v>561.038961038961</v>
+      </c>
+      <c r="C3415" t="n">
+        <v>9266.813073056701</v>
+      </c>
+      <c r="D3415" t="n">
+        <v>575.4834257727591</v>
+      </c>
+      <c r="E3415" t="n">
+        <v>-24.51657422724088</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
stake pool flows added, dates for dcrdata altered
</commit_message>
<xml_diff>
--- a/btc_blk_times.xlsx
+++ b/btc_blk_times.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3415"/>
+  <dimension ref="A1:E3418"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -58260,6 +58260,57 @@
         <v>-24.51657422724088</v>
       </c>
     </row>
+    <row r="3416">
+      <c r="A3416" s="1" t="n">
+        <v>3414</v>
+      </c>
+      <c r="B3416" t="n">
+        <v>587.7551020408164</v>
+      </c>
+      <c r="C3416" t="n">
+        <v>9993.75317685564</v>
+      </c>
+      <c r="D3416" t="n">
+        <v>576.6204520118262</v>
+      </c>
+      <c r="E3416" t="n">
+        <v>-23.37954798817384</v>
+      </c>
+    </row>
+    <row r="3417">
+      <c r="A3417" s="1" t="n">
+        <v>3415</v>
+      </c>
+      <c r="B3417" t="n">
+        <v>630.6569343065694</v>
+      </c>
+      <c r="C3417" t="n">
+        <v>9859.323604617181</v>
+      </c>
+      <c r="D3417" t="n">
+        <v>578.3642039039181</v>
+      </c>
+      <c r="E3417" t="n">
+        <v>-21.63579609608189</v>
+      </c>
+    </row>
+    <row r="3418">
+      <c r="A3418" s="1" t="n">
+        <v>3416</v>
+      </c>
+      <c r="B3418" t="n">
+        <v>635.2941176470588</v>
+      </c>
+      <c r="C3418" t="n">
+        <v>9577.33892238457</v>
+      </c>
+      <c r="D3418" t="n">
+        <v>578.2521590859909</v>
+      </c>
+      <c r="E3418" t="n">
+        <v>-21.74784091400909</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>